<commit_message>
Corrected the wrong info
</commit_message>
<xml_diff>
--- a/docs/GROUP - C Weekly Progress Report.xlsx
+++ b/docs/GROUP - C Weekly Progress Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cardiovascular-disease-prediction\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tirth\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420DB037-E333-4E52-A337-548A8A9BA6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD13FE3D-8D30-4270-BFD2-CB7F9E4104F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{8223AA31-6659-428F-A36B-A92BFE678B6C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{8223AA31-6659-428F-A36B-A92BFE678B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="81">
   <si>
     <t>Members</t>
   </si>
@@ -68,12 +68,6 @@
     <t xml:space="preserve"> https://github.com/rutul7802</t>
   </si>
   <si>
-    <t xml:space="preserve">YETUNDE SHITTU </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> https://github.com/whyteeth</t>
-  </si>
-  <si>
     <t xml:space="preserve">SWETHA TANIKONDA </t>
   </si>
   <si>
@@ -264,6 +258,27 @@
   </si>
   <si>
     <t>DECISION TREES AND KNN</t>
+  </si>
+  <si>
+    <t>MODEL TUNING - DATA DUPLICATION, GRIDSEARCHCV</t>
+  </si>
+  <si>
+    <t>SLIDES AND PPT</t>
+  </si>
+  <si>
+    <t>Week - 11</t>
+  </si>
+  <si>
+    <t>XGBOOST PARAMETER TUNING</t>
+  </si>
+  <si>
+    <t>LOGISTIC REGRESSION PARAMETER TUNING</t>
+  </si>
+  <si>
+    <t>GBM PARAMETER TUNING</t>
+  </si>
+  <si>
+    <t>CHANGING IN PARAMETERS TO GET ACCURATE RESULT</t>
   </si>
 </sst>
 </file>
@@ -343,7 +358,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="13">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -380,6 +395,9 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -433,20 +451,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D57AB53B-F699-4696-B86A-BE5D01D4904D}" name="Table1" displayName="Table1" ref="A15:H23" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A15:H23" xr:uid="{D57AB53B-F699-4696-B86A-BE5D01D4904D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D57AB53B-F699-4696-B86A-BE5D01D4904D}" name="Table1" displayName="Table1" ref="A15:I23" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A15:I23" xr:uid="{D57AB53B-F699-4696-B86A-BE5D01D4904D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A16:G23">
     <sortCondition ref="A15:A23"/>
   </sortState>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{ED33A48B-D1CE-41CD-8CC6-34812A592555}" name="Members" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{FDB5DA1A-7203-4A45-8FA8-E99AF10F1B82}" name="Week 1-3" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{2CC5A466-7EB6-4634-8895-952B59F7A66E}" name="Week - 4" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{E40FD174-8A88-45E3-A0CC-689EF08CFC0D}" name="Week-5" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{FDEE3588-2152-4E62-80C0-6D232F7A0ECE}" name="Week - 6" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{055F4438-72ED-4FC2-9ED7-A3D45A9258D5}" name="Week - 7" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{9344000E-B16C-4BB9-875A-8497E3935AE5}" name="Week - 9" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{0D15DCEC-B2C7-48FE-B361-91B8FDB7DAE3}" name="Week - 10" dataDxfId="2"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{ED33A48B-D1CE-41CD-8CC6-34812A592555}" name="Members" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{FDB5DA1A-7203-4A45-8FA8-E99AF10F1B82}" name="Week 1-3" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{2CC5A466-7EB6-4634-8895-952B59F7A66E}" name="Week - 4" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{E40FD174-8A88-45E3-A0CC-689EF08CFC0D}" name="Week-5" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{FDEE3588-2152-4E62-80C0-6D232F7A0ECE}" name="Week - 6" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{055F4438-72ED-4FC2-9ED7-A3D45A9258D5}" name="Week - 7" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{9344000E-B16C-4BB9-875A-8497E3935AE5}" name="Week - 9" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{0D15DCEC-B2C7-48FE-B361-91B8FDB7DAE3}" name="Week - 10" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{3E681203-D626-41A0-A13C-41B528BA7F22}" name="Week - 11" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -455,6 +474,9 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D6312D3B-786A-47CE-BE6B-AD57DB5CA6C6}" name="Table3" displayName="Table3" ref="A2:B11" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A2:B11" xr:uid="{D6312D3B-786A-47CE-BE6B-AD57DB5CA6C6}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B11">
+    <sortCondition ref="A2:A11"/>
+  </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{B2CE2999-A66A-4FBA-B83D-33D32E7E301E}" name="Members"/>
     <tableColumn id="2" xr3:uid="{E02ACA79-C341-474E-A4B4-3A9E9FE07FBC}" name="GitHub"/>
@@ -780,79 +802,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{964F5DAF-D7EF-4C3F-9A9D-DD7862803C73}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="E13" zoomScale="83" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="8"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
       <c r="B7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -860,7 +883,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -868,270 +891,289 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G15" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H16" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I16" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="G18" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+      <c r="I19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H22" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I22" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>50</v>
+        <v>41</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:B11">
+  <conditionalFormatting sqref="B3:B10">
     <cfRule type="uniqueValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" display="https://github.com/gaurav809" xr:uid="{9F0146CC-50CC-4F73-8935-41CD22CA3C83}"/>
-    <hyperlink ref="A5" r:id="rId2" display="https://github.com/tirth-patel01" xr:uid="{72DD30BD-5407-4824-AFB9-664AE4F9B048}"/>
-    <hyperlink ref="A11" r:id="rId3" display="https://github.com/amannain122" xr:uid="{1AC88A5A-887D-428B-92A3-69F80D6CA6FB}"/>
+    <hyperlink ref="A5" r:id="rId1" display="https://github.com/gaurav809" xr:uid="{9F0146CC-50CC-4F73-8935-41CD22CA3C83}"/>
+    <hyperlink ref="A10" r:id="rId2" display="https://github.com/tirth-patel01" xr:uid="{72DD30BD-5407-4824-AFB9-664AE4F9B048}"/>
+    <hyperlink ref="A3" r:id="rId3" display="https://github.com/amannain122" xr:uid="{1AC88A5A-887D-428B-92A3-69F80D6CA6FB}"/>
     <hyperlink ref="A18" r:id="rId4" display="https://github.com/gaurav809" xr:uid="{BF272794-3603-44A0-B19F-13312A27B917}"/>
     <hyperlink ref="A23" r:id="rId5" display="https://github.com/tirth-patel01" xr:uid="{98C89845-5CF5-43A5-80B5-F25DF17B3EC3}"/>
     <hyperlink ref="A16" r:id="rId6" display="https://github.com/amannain122" xr:uid="{8D7EB5B3-F8B7-4DCE-B367-2B5BB4254AE5}"/>

</xml_diff>

<commit_message>
Change the parameters to get more accurate result
</commit_message>
<xml_diff>
--- a/docs/GROUP - C Weekly Progress Report.xlsx
+++ b/docs/GROUP - C Weekly Progress Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College\Assignments\Steps\cardiovascular-disease-prediction\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33E9317-B4A9-4920-906C-B2475D2A6B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE33A72-C2A7-4A09-A19A-3ED2DB0C02E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{8223AA31-6659-428F-A36B-A92BFE678B6C}"/>
   </bookViews>
@@ -329,7 +329,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -337,12 +337,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -364,6 +401,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -817,7 +860,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="83" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A19" sqref="A19:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -974,31 +1017,31 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
+      </c>
+      <c r="I17" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -1031,32 +1074,32 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="I19" t="s">
-        <v>78</v>
+      <c r="A19" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -1147,32 +1190,32 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>4</v>
+      <c r="A23" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" t="s">
-        <v>56</v>
-      </c>
-      <c r="G23" t="s">
-        <v>66</v>
-      </c>
-      <c r="H23" t="s">
-        <v>66</v>
-      </c>
-      <c r="I23" t="s">
-        <v>80</v>
+        <v>27</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1187,7 +1230,7 @@
     <hyperlink ref="A10" r:id="rId2" display="https://github.com/tirth-patel01" xr:uid="{72DD30BD-5407-4824-AFB9-664AE4F9B048}"/>
     <hyperlink ref="A3" r:id="rId3" display="https://github.com/amannain122" xr:uid="{1AC88A5A-887D-428B-92A3-69F80D6CA6FB}"/>
     <hyperlink ref="A18" r:id="rId4" display="https://github.com/gaurav809" xr:uid="{BF272794-3603-44A0-B19F-13312A27B917}"/>
-    <hyperlink ref="A23" r:id="rId5" display="https://github.com/tirth-patel01" xr:uid="{98C89845-5CF5-43A5-80B5-F25DF17B3EC3}"/>
+    <hyperlink ref="A19" r:id="rId5" display="https://github.com/tirth-patel01" xr:uid="{98C89845-5CF5-43A5-80B5-F25DF17B3EC3}"/>
     <hyperlink ref="A16" r:id="rId6" display="https://github.com/amannain122" xr:uid="{8D7EB5B3-F8B7-4DCE-B367-2B5BB4254AE5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>